<commit_message>
Changed broadcasting from Broadcaster to Processor implementation, as the Processor implementation is more appropriate for asynchronous broadcasting. Also changed wiring up a Stream, now sharing an upstream pipeline and wiring up 2 downstream pipelines.
</commit_message>
<xml_diff>
--- a/output/reports/Measurements.xlsx
+++ b/output/reports/Measurements.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
     <sheet name="EDAPrimer" r:id="rId5" sheetId="2"/>
-    <sheet name="EDA" r:id="rId6" sheetId="3"/>
+    <sheet name="EDAPrimer2" r:id="rId6" sheetId="3"/>
   </sheets>
   <calcPr calcId="122211" calcOnSave="0"/>
 </workbook>
@@ -227,7 +227,7 @@
     <t>EDAPrimer</t>
   </si>
   <si>
-    <t>EDA</t>
+    <t>EDAPrimer2</t>
   </si>
 </sst>
 </file>
@@ -881,7 +881,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>87521.5</v>
+        <v>162388.0</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>12.901294498381876</v>
+        <v>19.671521035598705</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
@@ -982,16 +982,16 @@
         <v>0.0</v>
       </c>
       <c r="B12" t="n" s="0">
-        <v>77397.0</v>
+        <v>149127.0</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>700.0</v>
+        <v>1009.0</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>11.37378640776699</v>
+        <v>19.857605177993527</v>
       </c>
       <c r="F12" t="n" s="0">
         <v>0.0</v>
@@ -1035,16 +1035,16 @@
         <v>1.0</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>97646.0</v>
+        <v>143894.0</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>699.0</v>
+        <v>761.0</v>
       </c>
       <c r="D13" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>14.428802588996763</v>
+        <v>17.733009708737864</v>
       </c>
       <c r="F13" t="n" s="0">
         <v>0.0</v>
@@ -1080,6 +1080,165 @@
         <v>0.0</v>
       </c>
       <c r="Q13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.0" customHeight="true">
+      <c r="A14" t="n" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>162388.0</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>1088.0</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>19.218446601941746</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" ht="15.0" customHeight="true">
+      <c r="A15" t="n" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>181338.0</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>941.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>21.723300970873787</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.0" customHeight="true">
+      <c r="A16" t="n" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>182415.0</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>775.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>19.671521035598705</v>
+      </c>
+      <c r="F16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q16" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>
@@ -1138,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="B4" t="n" s="0">
-        <v>2941.5</v>
+        <v>165773.0</v>
       </c>
     </row>
     <row r="5" ht="15.0" customHeight="true">
@@ -1146,7 +1305,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="n" s="0">
-        <v>0.4285760517799353</v>
+        <v>18.681229773462782</v>
       </c>
     </row>
     <row r="6" ht="15.0" customHeight="true">
@@ -1239,16 +1398,16 @@
         <v>0.0</v>
       </c>
       <c r="B12" t="n" s="0">
-        <v>2977.0</v>
+        <v>165773.0</v>
       </c>
       <c r="C12" t="n" s="0">
-        <v>49.0</v>
+        <v>1132.0</v>
       </c>
       <c r="D12" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E12" t="n" s="0">
-        <v>0.4752750809061489</v>
+        <v>18.741100323624597</v>
       </c>
       <c r="F12" t="n" s="0">
         <v>0.0</v>
@@ -1292,16 +1451,16 @@
         <v>1.0</v>
       </c>
       <c r="B13" t="n" s="0">
-        <v>2906.0</v>
+        <v>174375.0</v>
       </c>
       <c r="C13" t="n" s="0">
-        <v>17.0</v>
+        <v>1399.0</v>
       </c>
       <c r="D13" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="E13" t="n" s="0">
-        <v>0.3818770226537217</v>
+        <v>19.45145631067961</v>
       </c>
       <c r="F13" t="n" s="0">
         <v>0.0</v>
@@ -1337,6 +1496,165 @@
         <v>0.0</v>
       </c>
       <c r="Q13" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="14" ht="15.0" customHeight="true">
+      <c r="A14" t="n" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="B14" t="n" s="0">
+        <v>166449.0</v>
+      </c>
+      <c r="C14" t="n" s="0">
+        <v>1119.0</v>
+      </c>
+      <c r="D14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="n" s="0">
+        <v>18.681229773462782</v>
+      </c>
+      <c r="F14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q14" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="15" ht="15.0" customHeight="true">
+      <c r="A15" t="n" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="B15" t="n" s="0">
+        <v>133298.0</v>
+      </c>
+      <c r="C15" t="n" s="0">
+        <v>668.0</v>
+      </c>
+      <c r="D15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="n" s="0">
+        <v>15.21359223300971</v>
+      </c>
+      <c r="F15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q15" t="n" s="0">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="16" ht="15.0" customHeight="true">
+      <c r="A16" t="n" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="B16" t="n" s="0">
+        <v>140785.0</v>
+      </c>
+      <c r="C16" t="n" s="0">
+        <v>715.0</v>
+      </c>
+      <c r="D16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="E16" t="n" s="0">
+        <v>17.401294498381876</v>
+      </c>
+      <c r="F16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="G16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="H16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="I16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="J16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="K16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="L16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="M16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="N16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="O16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="P16" t="n" s="0">
+        <v>0.0</v>
+      </c>
+      <c r="Q16" t="n" s="0">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>